<commit_message>
feat: melhorias e alterações
</commit_message>
<xml_diff>
--- a/TESTE.xlsx
+++ b/TESTE.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,35 +543,25 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>2025-01-30 03:27:15</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -591,6 +581,84 @@
       <c r="K3" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-01-30 11:22:54</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-01-30 11:49:51</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>em dia</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>em aberto</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>sim</t>
         </is>
       </c>
     </row>

</xml_diff>